<commit_message>
modified to support threadlocal
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\seleniumworkspaces\LiveProjects\DataDrivenFramework\src\test\resources\excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17205" windowHeight="5370" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17205" windowHeight="5370"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
@@ -17,8 +12,8 @@
     <sheet name="OpenAccountTest" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -103,8 +98,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,7 +190,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -230,7 +225,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -407,23 +402,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -431,7 +430,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -439,7 +438,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -447,7 +446,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -461,16 +460,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -487,7 +486,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -504,7 +503,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -521,7 +520,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -538,7 +537,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -561,16 +560,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -578,7 +577,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>10</v>
       </c>

</xml_diff>